<commit_message>
Uploaded 03-九月-2019 12:47:48 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FEF2DD-7655-C34D-BCE7-A466DB3D8A33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EA56F-6117-4245-85F3-A7E7F42983A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37540" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -59,6 +59,10 @@
     <t>CONDITION</t>
   </si>
   <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>$Insured: Insured</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +99,14 @@
   </si>
   <si>
     <t>blacklist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rule Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +140,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -216,7 +236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -248,10 +268,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,15 +594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDBB517-12D1-9B4E-80F7-8CBFF916DAE5}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,18 +659,18 @@
         <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -652,30 +679,28 @@
     <row r="7" spans="1:6">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="16">
-      <c r="A8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>10</v>
+    <row r="8" spans="1:6">
+      <c r="A8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="16">
       <c r="A9" s="12" t="s">
@@ -685,17 +710,33 @@
         <v>11</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" ht="16">
+      <c r="A10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded 03-九月-2019 12:55:33 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EA56F-6117-4245-85F3-A7E7F42983A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A655815A-BC32-9F45-A9A8-DE7C325BE603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37540" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -107,6 +107,10 @@
   </si>
   <si>
     <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RuleTable 黑名單</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -150,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +173,14 @@
         <bgColor rgb="FF94BD5E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6633"/>
+        <bgColor rgb="FFFF6633"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -230,55 +240,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,16 +649,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDBB517-12D1-9B4E-80F7-8CBFF916DAE5}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D10"/>
+      <selection activeCell="C9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,132 +668,144 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="16">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="16">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="16">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="9" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="16">
-      <c r="A9" s="12" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="16">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="16">
-      <c r="A10" s="12" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="16">
+      <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded 03-九月-2019 12:59:38 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A655815A-BC32-9F45-A9A8-DE7C325BE603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16220305-FF9E-3A41-BA05-DEF8BE88D3F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37540" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
@@ -90,10 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>拒保</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RULEFLOW-GROUP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,6 +107,10 @@
   </si>
   <si>
     <t>RuleTable 黑名單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"拒保"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -652,7 +652,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A9:C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -710,7 +710,7 @@
     </row>
     <row r="5" spans="1:6" ht="16">
       <c r="A5" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -729,7 +729,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -758,13 +758,13 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="6"/>
@@ -778,10 +778,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
@@ -794,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="6"/>

</xml_diff>

<commit_message>
Uploaded 03-九月-2019 14:05:29 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC70FE9E-17BD-C14F-809D-8B1F3B9C9F4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E31C26-9F88-C443-8E26-F70222D86436}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37540" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
+    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$Insured: Insured</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -80,10 +76,6 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>$Insured.setStatus($param)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RULEFLOW-GROUP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,6 +105,14 @@
   </si>
   <si>
     <t>blacklist-rule2</t>
+  </si>
+  <si>
+    <t>$insured: Insured</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$insured.setStatus($param);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDBB517-12D1-9B4E-80F7-8CBFF916DAE5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -711,7 +711,7 @@
     </row>
     <row r="5" spans="1:6" ht="16">
       <c r="A5" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -727,10 +727,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -738,7 +738,7 @@
     <row r="7" spans="1:6">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="10"/>
@@ -748,10 +748,10 @@
     <row r="8" spans="1:6">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="6"/>
@@ -759,13 +759,13 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="6"/>
@@ -773,29 +773,29 @@
     </row>
     <row r="10" spans="1:6" ht="16">
       <c r="A10" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="16">
       <c r="A11" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="6"/>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:22:48 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E31C26-9F88-C443-8E26-F70222D86436}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A813B41D-CF33-5043-92A1-1BF559C6F23F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.redhat.prudential_poc.pojo.Application,com.redhat.prudential_poc.pojo.Insured</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>黑名單check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,6 +108,10 @@
   </si>
   <si>
     <t>$insured.setStatus($param);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.pojo.Insured</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,7 +653,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -694,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -711,7 +711,7 @@
     </row>
     <row r="5" spans="1:6" ht="16">
       <c r="A5" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -721,16 +721,16 @@
     </row>
     <row r="6" spans="1:6" ht="16">
       <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -738,7 +738,7 @@
     <row r="7" spans="1:6">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="10"/>
@@ -748,10 +748,10 @@
     <row r="8" spans="1:6">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="6"/>
@@ -759,13 +759,13 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="6"/>
@@ -773,29 +773,29 @@
     </row>
     <row r="10" spans="1:6" ht="16">
       <c r="A10" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="16">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="6"/>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:25:25 {/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/BlackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A813B41D-CF33-5043-92A1-1BF559C6F23F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D911740-0B18-0945-B3FC-B15B101BED78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" xr2:uid="{BAEDE162-4390-CA4F-84BC-8544F53C142F}"/>
   </bookViews>
@@ -59,10 +59,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A223456123</t>
   </si>
   <si>
@@ -112,6 +108,10 @@
   </si>
   <si>
     <t>com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insuredId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,7 +653,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -711,7 +711,7 @@
     </row>
     <row r="5" spans="1:6" ht="16">
       <c r="A5" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -727,10 +727,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -738,7 +738,7 @@
     <row r="7" spans="1:6">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="10"/>
@@ -748,10 +748,10 @@
     <row r="8" spans="1:6">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="6"/>
@@ -759,13 +759,13 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="6"/>
@@ -773,29 +773,29 @@
     </row>
     <row r="10" spans="1:6" ht="16">
       <c r="A10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="16">
       <c r="A11" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="6"/>

</xml_diff>